<commit_message>
Add legend and conditional formatting to 2026 Excel file
Co-authored-by: pieter-1983 <24873242+pieter-1983@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Aanwezigheid Kantoor 2026.xlsx
+++ b/Aanwezigheid Kantoor 2026.xlsx
@@ -28,9 +28,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="d"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -41,7 +40,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -68,6 +67,41 @@
         <fgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249946592608417"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -81,17 +115,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249946592608417"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -453,7 +538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,97 +586,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46023</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46024</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46025</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46026</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46027</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46028</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46029</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46030</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46031</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46032</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46033</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46034</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46035</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46036</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46037</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46038</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46039</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46040</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46041</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46042</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46043</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46044</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46045</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46046</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46047</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46048</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46049</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46050</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46051</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46052</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46053</v>
       </c>
     </row>
@@ -1475,7 +1560,106 @@
       </c>
       <c r="AF12" s="2" t="n"/>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1486,7 +1670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1534,97 +1718,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46296</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46297</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46298</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46299</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46300</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46301</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46302</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46303</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46304</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46305</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46306</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46307</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46308</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46309</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46310</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46311</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46312</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46313</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46314</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46315</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46316</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46317</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46318</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46319</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46320</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46321</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46322</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46323</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46324</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46325</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46326</v>
       </c>
     </row>
@@ -2530,7 +2714,106 @@
       </c>
       <c r="AF12" s="2" t="n"/>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2541,7 +2824,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2588,94 +2871,94 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46327</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46328</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46329</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46330</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46331</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46332</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46333</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46334</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46335</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46336</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46337</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46338</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46339</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46340</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46341</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46342</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46343</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46344</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46345</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46346</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46347</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46348</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46349</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46350</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46351</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46352</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46353</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46354</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46355</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46356</v>
       </c>
     </row>
@@ -3526,7 +3809,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AE12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3537,7 +3919,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3585,97 +3967,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46357</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46358</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46359</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46360</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46361</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46362</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46363</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46364</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46365</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46366</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46367</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46368</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46369</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46370</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46371</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46372</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46373</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46374</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46375</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46376</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46377</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46378</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46379</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46380</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46381</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46382</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46383</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46384</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46385</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46386</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46387</v>
       </c>
     </row>
@@ -4581,7 +4963,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4592,7 +5073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A17:B20"/>
+  <dimension ref="A17:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4611,33 +5092,82 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
         <is>
           <t>Nee</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="inlineStr">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9" t="inlineStr">
         <is>
           <t>Misschien</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
         <is>
           <t>Onbekend</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>4</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -4651,7 +5181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:AC22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4696,88 +5226,88 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46054</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46055</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46056</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46057</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46058</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46059</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46060</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46061</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46062</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46063</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46064</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46065</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46066</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46067</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46068</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46069</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46070</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46071</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46072</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46073</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46074</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46075</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46076</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46077</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46078</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46079</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46080</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46081</v>
       </c>
     </row>
@@ -5606,7 +6136,106 @@
       </c>
       <c r="AC12" s="2" t="n"/>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AC12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5617,7 +6246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5665,97 +6294,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46082</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46083</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46084</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46085</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46086</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46087</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46088</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46089</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46090</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46091</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46092</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46093</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46094</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46095</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46096</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46097</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46098</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46099</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46100</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46101</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46102</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46103</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46104</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46105</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46106</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46107</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46108</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46109</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46110</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46111</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46112</v>
       </c>
     </row>
@@ -6661,7 +7290,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6672,7 +7400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6719,94 +7447,94 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46113</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46114</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46115</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46116</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46117</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46118</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46119</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46120</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46121</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46122</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46123</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46124</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46125</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46126</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46127</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46128</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46129</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46130</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46131</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46132</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46133</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46134</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46135</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46136</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46137</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46138</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46139</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46140</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46141</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46142</v>
       </c>
     </row>
@@ -7679,7 +8407,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AE12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7690,7 +8517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7738,97 +8565,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46143</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46144</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46145</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46146</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46147</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46148</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46149</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46150</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46151</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46152</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46153</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46154</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46155</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46156</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46157</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46158</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46159</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46160</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46161</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46162</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46163</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46164</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46165</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46166</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46167</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46168</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46169</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46170</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46171</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46172</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46173</v>
       </c>
     </row>
@@ -8646,7 +9473,106 @@
       <c r="AE12" s="2" t="n"/>
       <c r="AF12" s="2" t="n"/>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -8657,7 +9583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8704,94 +9630,94 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46174</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46175</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46176</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46177</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46178</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46179</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46180</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46181</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46182</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46183</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46184</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46185</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46186</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46187</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46188</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46189</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46190</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46191</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46192</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46193</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46194</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46195</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46196</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46197</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46198</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46199</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46200</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46201</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46202</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46203</v>
       </c>
     </row>
@@ -9686,7 +10612,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AE12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9697,7 +10722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9745,97 +10770,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46204</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46205</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46206</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46207</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46208</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46209</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46210</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46211</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46212</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46213</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46214</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46215</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46216</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46217</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46218</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46219</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46220</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46221</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46222</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46223</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46224</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46225</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46226</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46227</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46228</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46229</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46230</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46231</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46232</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46233</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46234</v>
       </c>
     </row>
@@ -10741,7 +11766,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -10752,7 +11876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10800,97 +11924,97 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46235</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46236</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46237</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46238</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46239</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46240</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46241</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46242</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46243</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46244</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46245</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46246</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46247</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46248</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46249</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46250</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46251</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46252</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46253</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46254</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46255</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46256</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46257</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46258</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46259</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46260</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46261</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46262</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46263</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46264</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="6" t="n">
         <v>46265</v>
       </c>
     </row>
@@ -11774,7 +12898,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AF12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -11785,7 +13008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11832,94 +13055,94 @@
           <t>Naam</t>
         </is>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="6" t="n">
         <v>46266</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="6" t="n">
         <v>46267</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="6" t="n">
         <v>46268</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="6" t="n">
         <v>46269</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="6" t="n">
         <v>46270</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="6" t="n">
         <v>46271</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="6" t="n">
         <v>46272</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="6" t="n">
         <v>46273</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="6" t="n">
         <v>46274</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="6" t="n">
         <v>46275</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="6" t="n">
         <v>46276</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="6" t="n">
         <v>46277</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="6" t="n">
         <v>46278</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="6" t="n">
         <v>46279</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="6" t="n">
         <v>46280</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="6" t="n">
         <v>46281</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="6" t="n">
         <v>46282</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="6" t="n">
         <v>46283</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="6" t="n">
         <v>46284</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="6" t="n">
         <v>46285</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="6" t="n">
         <v>46286</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="6" t="n">
         <v>46287</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="6" t="n">
         <v>46288</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="6" t="n">
         <v>46289</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="6" t="n">
         <v>46290</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="6" t="n">
         <v>46291</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="6" t="n">
         <v>46292</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="6" t="n">
         <v>46293</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="6" t="n">
         <v>46294</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="6" t="n">
         <v>46295</v>
       </c>
     </row>
@@ -12814,7 +14037,106 @@
         <v>4</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ja </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="inlineStr">
+        <is>
+          <t>Misschien</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>Aanwezig met fiets</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>Fiets klant</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AE12">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>